<commit_message>
Pridané DB funkcie implemenbtované do XLSX operatívnych funkcií (add,edit,delete).
Zvýšená rýchlosť načitavania.

Problémy - čítanie mena a emailu ako text na viac riadkov a aj pole, s koým treba pracvovať
</commit_message>
<xml_diff>
--- a/resources/1.xlsx
+++ b/resources/1.xlsx
@@ -16,24 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="5">
   <si>
-    <t>Rikon Ladňák</t>
+    <t>Dizajn 250€
+Webstránka 10515€
+Marináda 32€</t>
   </si>
   <si>
-    <t>Et kete</t>
+    <t>Erik Ladňák
+Jakub Rončák
+Elf René</t>
   </si>
   <si>
-    <t>Dizajn</t>
+    <t>ladnak.erik@gmail.com
+jakub.roncak@gmail.com
+elf@rene.sk</t>
   </si>
   <si>
-    <t>Webstránka</t>
+    <t>Poznámka na 
+viac riadkov</t>
   </si>
   <si>
-    <t>Marináda s kečupom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ladnak.erik@gmail.com </t>
+    <t>Dizajn 250€
+Webstránka 10    515€
+Marináda 32€</t>
   </si>
 </sst>
 </file>
@@ -73,7 +79,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,17 +87,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -397,7 +424,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,295 +432,158 @@
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6">
+        <v>43668</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43669</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2">
-        <v>43668</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3">
-        <v>250</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C3" s="6">
+        <v>43649</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3">
-        <v>1054500</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3">
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C4" s="6">
+        <v>43619</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43669</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
-        <v>251</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C5" s="6">
+        <v>43589</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
-        <v>1054501</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="3">
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43649</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>252</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C7" s="6">
+        <v>43551</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3">
-        <v>1054502</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="3">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="3">
-        <v>252</v>
-      </c>
-      <c r="N3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1054502</v>
-      </c>
-      <c r="P3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>43619</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>253</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1054503</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="3">
-        <v>5</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3">
-        <v>253</v>
-      </c>
-      <c r="N4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="3">
-        <v>1054503</v>
-      </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>43589</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>254</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1054504</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="3">
-        <v>6</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="3">
-        <v>254</v>
-      </c>
-      <c r="N5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="3">
-        <v>1054504</v>
-      </c>
-      <c r="P5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>43559</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>255</v>
-      </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1054505</v>
-      </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>43551</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3">
-        <v>256</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1054506</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="3">
-        <v>8</v>
-      </c>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -726,7 +616,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1" display="ladnak.erik@gmail.com "/>
     <hyperlink ref="B2:B7" r:id="rId2" display="ladnak.erik@gmail.com "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>